<commit_message>
Modified based on the CR 1
Changes made to FirstPowerBi Report - Changes Stacked bar chart to Stacked column chart
Changes made to Family_Expenses_Daily_Data - Added 1 row in the last
Changes made to Case study - Added Word Test and Data prefix to Sources
</commit_message>
<xml_diff>
--- a/Family_Expenses_Daily_Data.xlsx
+++ b/Family_Expenses_Daily_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VINAYTECH_POWER BI_FILES_DATABASES_BACKUP_RESTORE_DOC\GENERAL FILES FOR PRACTICE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagal\Downloads\kiran_7pm_NewRep-Dev\kiran_7pm_NewRep-Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BD255A-7073-46E4-99EB-E26E050B3271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1CE2CC-9B5A-40F7-AA51-156A9E936A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -232,9 +232,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -272,9 +272,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -307,26 +307,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -359,26 +342,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -552,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1958,6 +1924,23 @@
         <v>33</v>
       </c>
       <c r="E82" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>43657</v>
+      </c>
+      <c r="B83">
+        <v>400</v>
+      </c>
+      <c r="C83" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83" t="s">
+        <v>19</v>
+      </c>
+      <c r="E83" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>